<commit_message>
Add all arithmetic instructions
</commit_message>
<xml_diff>
--- a/tst/chip8Func.xlsx
+++ b/tst/chip8Func.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="129">
   <si>
     <t>0NNN</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1067,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,8 +1405,12 @@
       <c r="D17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1418,8 +1425,12 @@
       <c r="D18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -1434,8 +1445,12 @@
       <c r="D19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -1450,8 +1465,12 @@
       <c r="D20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">

</xml_diff>